<commit_message>
Saved my local changes before pulling updates
</commit_message>
<xml_diff>
--- a/ACCOUNT/Account__123456.xlsx
+++ b/ACCOUNT/Account__123456.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -506,7 +506,7 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>BALANCE : 6399.0</t>
+          <t>BALANCE : 6398.0</t>
         </is>
       </c>
     </row>
@@ -656,6 +656,24 @@
       </c>
       <c r="D18" t="n">
         <v>6399</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2025-10-22 20:00:21</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Withdraw</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" t="n">
+        <v>6398</v>
       </c>
     </row>
   </sheetData>

</xml_diff>